<commit_message>
Ten imputations instead of five
</commit_message>
<xml_diff>
--- a/Development/Results/flexibility.xlsx
+++ b/Development/Results/flexibility.xlsx
@@ -23,61 +23,61 @@
     <t xml:space="preserve">dPTH + CorrCa24u + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">190.5</t>
+    <t xml:space="preserve">182.7</t>
   </si>
   <si>
     <t xml:space="preserve">rms::rcs(dPTH, 3) + CorrCa24u + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">191.6</t>
+    <t xml:space="preserve">183.9</t>
   </si>
   <si>
     <t xml:space="preserve">rms::rcs(dPTH, 4) + CorrCa24u + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">190.3</t>
+    <t xml:space="preserve">182.4</t>
   </si>
   <si>
     <t xml:space="preserve">rms::rcs(dPTH, 5) + CorrCa24u + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">191.8</t>
+    <t xml:space="preserve">184.9</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + rms::rcs(CorrCa24u, 3) + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">192.0</t>
+    <t xml:space="preserve">184.1</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + rms::rcs(CorrCa24u, 4) + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">193.9</t>
+    <t xml:space="preserve">185.9</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + rms::rcs(CorrCa24u, 5) + Age_Years</t>
   </si>
   <si>
-    <t xml:space="preserve">195.8</t>
+    <t xml:space="preserve">187.6</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + CorrCa24u + rms::rcs(Age_Years, 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">191.3</t>
+    <t xml:space="preserve">183.8</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + CorrCa24u + rms::rcs(Age_Years, 4)</t>
   </si>
   <si>
-    <t xml:space="preserve">193.2</t>
+    <t xml:space="preserve">185.8</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + CorrCa24u + rms::rcs(Age_Years, 5)</t>
   </si>
   <si>
-    <t xml:space="preserve">192.1</t>
+    <t xml:space="preserve">185.0</t>
   </si>
   <si>
     <t xml:space="preserve">rms::rcs(dPTH, 4) + rms::rcs(CorrCa24u, 3) + Age_Years</t>
@@ -86,19 +86,19 @@
     <t xml:space="preserve">rms::rcs(dPTH, 4) + CorrCa24u + rms::rcs(Age_Years, 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">191.2</t>
+    <t xml:space="preserve">183.7</t>
   </si>
   <si>
     <t xml:space="preserve">dPTH + rms::rcs(CorrCa24u, 3) + rms::rcs(Age_Years, 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">192.6</t>
+    <t xml:space="preserve">185.1</t>
   </si>
   <si>
     <t xml:space="preserve">rms::rcs(dPTH, 4) + rms::rcs(CorrCa24u, 3) + rms::rcs(Age_Years, 3)</t>
   </si>
   <si>
-    <t xml:space="preserve">192.8</t>
+    <t xml:space="preserve">185.3</t>
   </si>
 </sst>
 </file>

</xml_diff>